<commit_message>
MoveTexture + background GameBounds fix / Clamp Move Player Player Move Normalize
</commit_message>
<xml_diff>
--- a/PewPewSource/Assets/ROADMAP.xlsx
+++ b/PewPewSource/Assets/ROADMAP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="28455" windowHeight="12795" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="28455" windowHeight="12795"/>
   </bookViews>
   <sheets>
     <sheet name="ROADMAP" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="184">
   <si>
     <t>Switch Ammo</t>
   </si>
@@ -570,10 +570,7 @@
     <t>TODO TMP</t>
   </si>
   <si>
-    <t>Améliorer Camera</t>
-  </si>
-  <si>
-    <t>Player Bounds to Cam</t>
+    <t>!</t>
   </si>
 </sst>
 </file>
@@ -975,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23.25"/>
@@ -1012,7 +1009,7 @@
         <v>112</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1032,15 +1029,24 @@
       <c r="C6" t="s">
         <v>116</v>
       </c>
+      <c r="D6" s="7" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="C7" t="s">
         <v>117</v>
       </c>
+      <c r="D7" s="7" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="C8" t="s">
         <v>118</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2087,10 +2093,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2103,16 +2109,6 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>184</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Move Controll EnemyController.cs FireRate CD Internal Gameloop sequence logic
</commit_message>
<xml_diff>
--- a/PewPewSource/Assets/ROADMAP.xlsx
+++ b/PewPewSource/Assets/ROADMAP.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="185">
   <si>
     <t>Switch Ammo</t>
   </si>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t>!</t>
+  </si>
+  <si>
+    <t>Order AI / MOVE / Body / Shot</t>
   </si>
 </sst>
 </file>
@@ -972,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23.25"/>
@@ -1061,6 +1064,9 @@
       <c r="C11" t="s">
         <v>120</v>
       </c>
+      <c r="D11" s="7" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" s="5" t="s">
@@ -1225,12 +1231,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="C49" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:4">
       <c r="B51" s="5" t="s">
         <v>87</v>
       </c>
@@ -1238,7 +1244,15 @@
         <v>161</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="52" spans="1:4">
+      <c r="C52" t="s">
+        <v>184</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="4" t="s">
         <v>163</v>
       </c>
@@ -1249,17 +1263,17 @@
         <v>164</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:4">
       <c r="C55" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:4">
       <c r="C56" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:4">
       <c r="B57" s="5" t="s">
         <v>8</v>
       </c>
@@ -1267,37 +1281,37 @@
         <v>167</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:4">
       <c r="C58" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:4">
       <c r="C59" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:4">
       <c r="C60" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:4">
       <c r="C61" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:4">
       <c r="C62" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:4">
       <c r="C63" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:4">
       <c r="C64" t="s">
         <v>173</v>
       </c>

</xml_diff>

<commit_message>
Add immortal + duration
</commit_message>
<xml_diff>
--- a/PewPewSource/Assets/ROADMAP.xlsx
+++ b/PewPewSource/Assets/ROADMAP.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="185">
   <si>
     <t>Switch Ammo</t>
   </si>
@@ -975,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23.25"/>
@@ -1075,10 +1075,16 @@
       <c r="C13" t="s">
         <v>10</v>
       </c>
+      <c r="D13" s="7" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="C14" t="s">
         <v>122</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:4">

</xml_diff>

<commit_message>
Add Curve Mode to movecomponent Refacto fct move
</commit_message>
<xml_diff>
--- a/PewPewSource/Assets/ROADMAP.xlsx
+++ b/PewPewSource/Assets/ROADMAP.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="185">
   <si>
     <t>Switch Ammo</t>
   </si>
@@ -975,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23.25"/>
@@ -1095,7 +1095,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:4">
       <c r="B18" s="5" t="s">
         <v>124</v>
       </c>
@@ -1103,17 +1103,17 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:4">
       <c r="C19" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:4">
       <c r="C20" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:4">
       <c r="B22" s="5" t="s">
         <v>128</v>
       </c>
@@ -1121,35 +1121,38 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:4">
       <c r="C23" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:4">
       <c r="C24" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:4">
       <c r="B26" s="5" t="s">
         <v>92</v>
       </c>
       <c r="C26" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="27" spans="2:3">
+      <c r="D26" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
       <c r="C27" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:4">
       <c r="C28" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:4">
       <c r="B30" s="5" t="s">
         <v>134</v>
       </c>

</xml_diff>

<commit_message>
Event / Respawn Player Add Direction
</commit_message>
<xml_diff>
--- a/PewPewSource/Assets/ROADMAP.xlsx
+++ b/PewPewSource/Assets/ROADMAP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="28455" windowHeight="12795"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="28455" windowHeight="12795" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ROADMAP" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="191">
   <si>
     <t>Switch Ammo</t>
   </si>
@@ -574,6 +574,24 @@
   </si>
   <si>
     <t>Order AI / MOVE / Body / Shot</t>
+  </si>
+  <si>
+    <t>Utilité réel ?</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Pas pour l'instant</t>
+  </si>
+  <si>
+    <t>Faire les spawner</t>
+  </si>
+  <si>
+    <t>Score module</t>
+  </si>
+  <si>
+    <t>Commencer qq AI</t>
   </si>
 </sst>
 </file>
@@ -973,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23.25"/>
@@ -985,6 +1003,7 @@
     <col min="2" max="2" width="41.42578125" style="5" customWidth="1"/>
     <col min="3" max="3" width="97.140625" customWidth="1"/>
     <col min="4" max="4" width="35.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="61.5" customHeight="1">
@@ -1094,8 +1113,11 @@
       <c r="C16" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="18" spans="2:4">
+      <c r="D16" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
       <c r="B18" s="5" t="s">
         <v>124</v>
       </c>
@@ -1103,17 +1125,17 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:5">
       <c r="C19" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:5">
       <c r="C20" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:5">
       <c r="B22" s="5" t="s">
         <v>128</v>
       </c>
@@ -1121,17 +1143,17 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:5">
       <c r="C23" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:5">
       <c r="C24" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:5">
       <c r="B26" s="5" t="s">
         <v>92</v>
       </c>
@@ -1142,22 +1164,31 @@
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:5">
       <c r="C27" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="28" spans="2:4">
+      <c r="E27" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
       <c r="C28" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="30" spans="2:4">
+      <c r="D28" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
       <c r="B30" s="5" t="s">
         <v>134</v>
       </c>
       <c r="C30" t="s">
         <v>135</v>
+      </c>
+      <c r="E30" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1275,6 +1306,9 @@
     <row r="55" spans="1:4">
       <c r="C55" t="s">
         <v>165</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2116,10 +2150,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2132,6 +2166,21 @@
         <v>182</v>
       </c>
     </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>190</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>